<commit_message>
almost all done edit part is pending
</commit_message>
<xml_diff>
--- a/data/inventory_data.xlsx
+++ b/data/inventory_data.xlsx
@@ -7,11 +7,11 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="customers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="purchases" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="inventory" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="products" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="vendors" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="purchases" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="customers" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="vendors" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="sales" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,65 +441,104 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Customer_ID</t>
+          <t>HSN_Code</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Product_Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Vendor</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Address</t>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Units</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Cost_per_Unit</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total_Cost</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Harsh</t>
+          <t>Keyboard</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>h@gmail.com</t>
+          <t>Amit</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mumbai</t>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1200</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>120000</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jay</t>
+          <t>mouse</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>j@gmail.com</t>
+          <t>Amit</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bihari</t>
-        </is>
+          <t>2025-06-08</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>21</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2200</v>
+      </c>
+      <c r="G3" t="n">
+        <v>46200</v>
       </c>
     </row>
   </sheetData>
@@ -605,6 +644,47 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Customer_ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -642,62 +722,6 @@
       <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>HSN_Code</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Product_Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Vendor</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Units</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Cost_per_Unit</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Total_Cost</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
changed the data in xlsx file
</commit_message>
<xml_diff>
--- a/data/inventory_data.xlsx
+++ b/data/inventory_data.xlsx
@@ -2,33 +2,37 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="purchases" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="inventory" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="products" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="customers" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="vendors" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="inventory" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="products" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="customers" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="vendors" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="purchases" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="sales" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -42,12 +46,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -60,14 +79,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -430,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,39 +461,34 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>HSN_Code</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Product_Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Vendor</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Cost_per_Unit</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Total_Cost</t>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Cost</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Selling_Price</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Total_cost</t>
         </is>
       </c>
     </row>
@@ -483,62 +500,68 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Keyboard</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Amit</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2025-06-08</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>120000</t>
-        </is>
+          <t>keyboard</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>14</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F2" t="n">
+        <v>28800</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>mouse</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Amit</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-06-08</t>
-        </is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2500</v>
       </c>
       <c r="E3" t="n">
-        <v>21</v>
+        <v>2700</v>
       </c>
       <c r="F3" t="n">
-        <v>2200</v>
-      </c>
-      <c r="G3" t="n">
-        <v>46200</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Pen</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -552,13 +575,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -573,23 +596,61 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Units</t>
+          <t>Cost</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Cost</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
           <t>Selling_Price</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Total_cost</t>
-        </is>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>keyboard</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Pen</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>15</v>
+      </c>
+      <c r="D4" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -603,33 +664,75 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>HSN_Code</t>
+          <t>Customer_ID</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Product_Name</t>
+          <t>Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Cost</t>
+          <t>Email</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Selling_Price</t>
+          <t>Address</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Harsh</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>h@gmail.com</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Jay</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>j@gmail.com</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Bihar</t>
         </is>
       </c>
     </row>
@@ -644,7 +747,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -653,24 +756,94 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Customer_ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>HSN_Code</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Vendor_Name</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Product_Name</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Phone</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Address</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Yash</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>keyboard</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>8989898989</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>y@gmail.com</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>UP</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Amit</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>7878787878</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>a@gmail.com</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>MP</t>
         </is>
       </c>
     </row>
@@ -685,7 +858,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -694,35 +867,71 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>HSN_Code</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Vendor_Name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Product_Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Phone</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Address</t>
-        </is>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Vendor</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Units</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Cost_per_Unit</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Total_Cost</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>keyboard</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Amit</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G2" t="n">
+        <v>14400</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +945,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -745,40 +954,71 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>HSN_Code</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>Product_Name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Customer</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="2" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="2" t="inlineStr">
         <is>
           <t>Selling_Price_per_Unit</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="2" t="inlineStr">
         <is>
           <t>Total_Amount</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>keyboard</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1 - Harsh</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G2" t="n">
+        <v>12000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now only edit purchase and sale should update the inventory part remain and also delete part as well
</commit_message>
<xml_diff>
--- a/data/inventory_data.xlsx
+++ b/data/inventory_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" tabRatio="600" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="inventory" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,7 +21,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -34,9 +34,6 @@
       <b val="1"/>
       <sz val="11"/>
     </font>
-    <font>
-      <b val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -46,7 +43,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -69,22 +66,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -458,45 +446,43 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>HSN_Code</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Product_Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Cost</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Selling_Price</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Total_cost</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -504,7 +490,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>14</v>
+        <v>1012</v>
       </c>
       <c r="D2" t="n">
         <v>1200</v>
@@ -513,14 +499,12 @@
         <v>1200</v>
       </c>
       <c r="F2" t="n">
-        <v>28800</v>
+        <v>1214400</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -528,23 +512,21 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D3" t="n">
-        <v>2500</v>
+        <v>2700</v>
       </c>
       <c r="E3" t="n">
         <v>2700</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>270000</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="A4" t="n">
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -578,7 +560,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -715,10 +697,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -732,7 +712,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bihar</t>
+          <t>Bihari</t>
         </is>
       </c>
     </row>
@@ -753,35 +733,35 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>HSN_Code</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Vendor_Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Product_Name</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Phone</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Email</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Address</t>
         </is>
@@ -816,10 +796,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -831,10 +809,8 @@
           <t>Mouse</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>7878787878</t>
-        </is>
+      <c r="D3" t="n">
+        <v>7878787878</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -858,80 +834,107 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>HSN_Code</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Product_Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Vendor</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Cost_per_Unit</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Total_Cost</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Yash</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-06-09</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>100</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2700</v>
+      </c>
+      <c r="G2" t="n">
+        <v>270000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>keyboard</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Amit</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>2025-06-09</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>12</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="E3" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F3" t="n">
         <v>1200</v>
       </c>
-      <c r="G2" t="n">
-        <v>14400</v>
+      <c r="G3" t="n">
+        <v>1200000</v>
       </c>
     </row>
   </sheetData>
@@ -951,50 +954,48 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>HSN_Code</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Product_Name</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Customer</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Units</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Selling_Price_per_Unit</t>
         </is>
       </c>
-      <c r="G1" s="2" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Total_Amount</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="A2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>

</xml_diff>